<commit_message>
Updates after review and restructuring for the new semester
</commit_message>
<xml_diff>
--- a/models_comp_comm/documents/Memory.xlsx
+++ b/models_comp_comm/documents/Memory.xlsx
@@ -678,7 +678,7 @@
       </c>
       <c r="D7" s="6">
         <f t="shared" ref="D7:D106" si="2">RANDBETWEEN(1,100)</f>
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1">
         <v>2.147483747E9</v>
@@ -694,7 +694,7 @@
       </c>
       <c r="D8" s="6">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1">
         <v>2.147483746E9</v>
@@ -710,7 +710,7 @@
       </c>
       <c r="D9" s="6">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="F9" s="1">
         <v>2.147483745E9</v>
@@ -726,7 +726,7 @@
       </c>
       <c r="D10" s="6">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1">
         <v>2.147483744E9</v>
@@ -742,7 +742,7 @@
       </c>
       <c r="D11" s="6">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="F11" s="1">
         <v>2.147483743E9</v>
@@ -758,7 +758,7 @@
       </c>
       <c r="D12" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="F12" s="1">
         <v>2.147483742E9</v>
@@ -774,7 +774,7 @@
       </c>
       <c r="D13" s="6">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F13" s="1">
         <v>2.147483741E9</v>
@@ -790,7 +790,7 @@
       </c>
       <c r="D14" s="6">
         <f t="shared" si="2"/>
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="F14" s="1">
         <v>2.14748374E9</v>
@@ -806,7 +806,7 @@
       </c>
       <c r="D15" s="6">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="1">
         <v>2.147483739E9</v>
@@ -822,7 +822,7 @@
       </c>
       <c r="D16" s="6">
         <f t="shared" si="2"/>
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="F16" s="1">
         <v>2.147483738E9</v>
@@ -838,7 +838,7 @@
       </c>
       <c r="D17" s="6">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F17" s="1">
         <v>2.147483737E9</v>
@@ -854,7 +854,7 @@
       </c>
       <c r="D18" s="6">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="F18" s="1">
         <v>2.147483736E9</v>
@@ -870,7 +870,7 @@
       </c>
       <c r="D19" s="6">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="F19" s="1">
         <v>2.147483735E9</v>
@@ -886,7 +886,7 @@
       </c>
       <c r="D20" s="6">
         <f t="shared" si="2"/>
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="F20" s="1">
         <v>2.147483734E9</v>
@@ -902,7 +902,7 @@
       </c>
       <c r="D21" s="6">
         <f t="shared" si="2"/>
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="F21" s="1">
         <v>2.147483733E9</v>
@@ -918,7 +918,7 @@
       </c>
       <c r="D22" s="6">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F22" s="1">
         <v>2.147483732E9</v>
@@ -934,7 +934,7 @@
       </c>
       <c r="D23" s="6">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="F23" s="1">
         <v>2.147483731E9</v>
@@ -966,7 +966,7 @@
       </c>
       <c r="D25" s="6">
         <f t="shared" si="2"/>
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="F25" s="1">
         <v>2.147483729E9</v>
@@ -982,7 +982,7 @@
       </c>
       <c r="D26" s="6">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="F26" s="1">
         <v>2.147483728E9</v>
@@ -998,7 +998,7 @@
       </c>
       <c r="D27" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F27" s="1">
         <v>2.147483727E9</v>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="D28" s="6">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="F28" s="1">
         <v>2.147483726E9</v>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="D29" s="6">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="F29" s="1">
         <v>2.147483725E9</v>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D30" s="6">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="F30" s="1">
         <v>2.147483724E9</v>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="D31" s="6">
         <f t="shared" si="2"/>
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="F31" s="1">
         <v>2.147483723E9</v>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="D32" s="6">
         <f t="shared" si="2"/>
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="F32" s="1">
         <v>2.147483722E9</v>
@@ -1094,7 +1094,7 @@
       </c>
       <c r="D33" s="6">
         <f t="shared" si="2"/>
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="F33" s="1">
         <v>2.147483721E9</v>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="D34" s="6">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="F34" s="1">
         <v>2.14748372E9</v>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="D35" s="6">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="F35" s="1">
         <v>2.147483719E9</v>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="D36" s="6">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="F36" s="1">
         <v>2.147483718E9</v>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="D37" s="6">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="F37" s="1">
         <v>2.147483717E9</v>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="D38" s="6">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F38" s="1">
         <v>2.147483716E9</v>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="D39" s="6">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F39" s="1">
         <v>2.147483715E9</v>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="D40" s="6">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="F40" s="1">
         <v>2.147483714E9</v>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="D41" s="6">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="F41" s="1">
         <v>2.147483713E9</v>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="D42" s="6">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F42" s="1">
         <v>2.147483712E9</v>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="D43" s="6">
         <f t="shared" si="2"/>
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="F43" s="1">
         <v>2.147483711E9</v>
@@ -1270,7 +1270,7 @@
       </c>
       <c r="D44" s="6">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="F44" s="1">
         <v>2.14748371E9</v>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="D45" s="6">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="F45" s="1">
         <v>2.147483709E9</v>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="D47" s="6">
         <f t="shared" si="2"/>
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="F47" s="1">
         <v>2.147483707E9</v>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="D48" s="6">
         <f t="shared" si="2"/>
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="F48" s="1">
         <v>2.147483706E9</v>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="D49" s="6">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="F49" s="1">
         <v>2.147483705E9</v>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="D50" s="6">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F50" s="1">
         <v>2.147483704E9</v>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="D51" s="6">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="F51" s="1">
         <v>2.147483703E9</v>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="D52" s="6">
         <f t="shared" si="2"/>
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="F52" s="1">
         <v>2.147483702E9</v>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="D53" s="6">
         <f t="shared" si="2"/>
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="F53" s="1">
         <v>2.147483701E9</v>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="D54" s="6">
         <f t="shared" si="2"/>
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="F54" s="1">
         <v>2.1474837E9</v>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="D55" s="6">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="F55" s="1">
         <v>2.147483699E9</v>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="D56" s="6">
         <f t="shared" si="2"/>
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="F56" s="1">
         <v>2.147483698E9</v>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="D57" s="6">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="F57" s="1">
         <v>2.147483697E9</v>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="D58" s="6">
         <f t="shared" si="2"/>
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="F58" s="1">
         <v>2.147483696E9</v>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="D59" s="6">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="F59" s="1">
         <v>2.147483695E9</v>
@@ -1526,7 +1526,7 @@
       </c>
       <c r="D60" s="6">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F60" s="1">
         <v>2.147483694E9</v>
@@ -1542,7 +1542,7 @@
       </c>
       <c r="D61" s="6">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="F61" s="1">
         <v>2.147483693E9</v>
@@ -1558,7 +1558,7 @@
       </c>
       <c r="D62" s="6">
         <f t="shared" si="2"/>
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="F62" s="1">
         <v>2.147483692E9</v>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="D63" s="6">
         <f t="shared" si="2"/>
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F63" s="1">
         <v>2.147483691E9</v>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="D64" s="6">
         <f t="shared" si="2"/>
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="F64" s="1">
         <v>2.14748369E9</v>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="D65" s="6">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="F65" s="1">
         <v>2.147483689E9</v>
@@ -1622,7 +1622,7 @@
       </c>
       <c r="D66" s="6">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F66" s="1">
         <v>2.147483688E9</v>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="D67" s="6">
         <f t="shared" si="2"/>
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F67" s="1">
         <v>2.147483687E9</v>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="D68" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F68" s="1">
         <v>2.147483686E9</v>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="D69" s="6">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="F69" s="1">
         <v>2.147483685E9</v>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="D70" s="6">
         <f t="shared" si="2"/>
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F70" s="1">
         <v>2.147483684E9</v>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="D71" s="6">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="F71" s="1">
         <v>2.147483683E9</v>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="D72" s="6">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F72" s="1">
         <v>2.147483682E9</v>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="D73" s="6">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="F73" s="1">
         <v>2.147483681E9</v>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="D74" s="6">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="F74" s="1">
         <v>2.14748368E9</v>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="D75" s="6">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="F75" s="1">
         <v>2.147483679E9</v>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="D76" s="6">
         <f t="shared" si="2"/>
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="F76" s="1">
         <v>2.147483678E9</v>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="D77" s="6">
         <f t="shared" si="2"/>
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F77" s="1">
         <v>2.147483677E9</v>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="D78" s="6">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="F78" s="1">
         <v>2.147483676E9</v>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="D79" s="6">
         <f t="shared" si="2"/>
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="F79" s="1">
         <v>2.147483675E9</v>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="D80" s="6">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F80" s="1">
         <v>2.147483674E9</v>
@@ -1862,7 +1862,7 @@
       </c>
       <c r="D81" s="6">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F81" s="1">
         <v>2.147483673E9</v>
@@ -1878,7 +1878,7 @@
       </c>
       <c r="D82" s="6">
         <f t="shared" si="2"/>
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="F82" s="1">
         <v>2.147483672E9</v>
@@ -1894,7 +1894,7 @@
       </c>
       <c r="D83" s="6">
         <f t="shared" si="2"/>
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="F83" s="1">
         <v>2.147483671E9</v>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="D84" s="6">
         <f t="shared" si="2"/>
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F84" s="1">
         <v>2.14748367E9</v>
@@ -1926,7 +1926,7 @@
       </c>
       <c r="D85" s="6">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="F85" s="1">
         <v>2.147483669E9</v>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="D86" s="6">
         <f t="shared" si="2"/>
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="F86" s="1">
         <v>2.147483668E9</v>
@@ -1958,7 +1958,7 @@
       </c>
       <c r="D87" s="6">
         <f t="shared" si="2"/>
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="F87" s="1">
         <v>2.147483667E9</v>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="D88" s="6">
         <f t="shared" si="2"/>
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="F88" s="1">
         <v>2.147483666E9</v>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="D89" s="6">
         <f t="shared" si="2"/>
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="F89" s="1">
         <v>2.147483665E9</v>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="D90" s="6">
         <f t="shared" si="2"/>
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="F90" s="1">
         <v>2.147483664E9</v>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D91" s="6">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F91" s="1">
         <v>2.147483663E9</v>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="D92" s="6">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="F92" s="1">
         <v>2.147483662E9</v>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="D93" s="6">
         <f t="shared" si="2"/>
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="F93" s="1">
         <v>2.147483661E9</v>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="D94" s="6">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F94" s="1">
         <v>2.14748366E9</v>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="D95" s="6">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F95" s="1">
         <v>2.147483659E9</v>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="D96" s="6">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="F96" s="1">
         <v>2.147483658E9</v>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="D97" s="6">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="F97" s="1">
         <v>2.147483657E9</v>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="D98" s="6">
         <f t="shared" si="2"/>
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="F98" s="1">
         <v>2.147483656E9</v>
@@ -2150,7 +2150,7 @@
       </c>
       <c r="D99" s="6">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="F99" s="1">
         <v>2.147483655E9</v>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="D100" s="6">
         <f t="shared" si="2"/>
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="F100" s="1">
         <v>2.147483654E9</v>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="D101" s="6">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="F101" s="1">
         <v>2.147483653E9</v>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="D102" s="6">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="F102" s="1">
         <v>2.147483652E9</v>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="D103" s="6">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="F103" s="1">
         <v>2.147483651E9</v>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="D104" s="6">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F104" s="1">
         <v>2.14748365E9</v>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="D105" s="6">
         <f t="shared" si="2"/>
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="F105" s="1">
         <v>2.147483649E9</v>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="D106" s="6">
         <f t="shared" si="2"/>
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="F106" s="1">
         <v>2.147483648E9</v>

</xml_diff>